<commit_message>
CTS-1000 added the RACI
</commit_message>
<xml_diff>
--- a/src/downloads/MOD-content-audit-template-OFFICIAL.xlsx
+++ b/src/downloads/MOD-content-audit-template-OFFICIAL.xlsx
@@ -10,7 +10,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="NolKtjNhFIMSKXZkShVsAIhtsQploI6jUaq5k+YJmIc="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="03wmL1NBd/uo7bm6feukQfGyQYDt70WYIaLP28Kwjqc="/>
     </ext>
   </extLst>
 </workbook>
@@ -44,7 +44,7 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t xml:space="preserve"> Save this in a place that everyone who needs access can get to it.
+      <t xml:space="preserve"> Save this in a shared folder so your team can access it. 
 </t>
     </r>
     <r>
@@ -307,14 +307,14 @@
     <t>Add any notes you want</t>
   </si>
   <si>
-    <t>You can recommend that content stays as it is or that changes are made.</t>
+    <t>You can recommend that the content stays as it is or that changes are made.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -339,7 +339,15 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -370,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="8">
     <border/>
     <border>
       <left/>
@@ -380,25 +388,7 @@
       <top/>
     </border>
     <border>
-      <right/>
-      <top/>
-    </border>
-    <border>
       <left/>
-    </border>
-    <border>
-      <right/>
-    </border>
-    <border>
-      <left/>
-      <bottom/>
-    </border>
-    <border>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -444,76 +434,62 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="12" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="12" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="14" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="13" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,152 +728,96 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="4"/>
-      <c r="K5" s="5"/>
+      <c r="B5" s="3"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="4"/>
-      <c r="K6" s="5"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="4"/>
-      <c r="K7" s="5"/>
+      <c r="B7" s="3"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="4"/>
-      <c r="K8" s="5"/>
+      <c r="B8" s="3"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="4"/>
-      <c r="K9" s="5"/>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="4"/>
-      <c r="K10" s="5"/>
+      <c r="B10" s="3"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="4"/>
-      <c r="K11" s="5"/>
+      <c r="B11" s="3"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="B12" s="4"/>
-      <c r="K12" s="5"/>
+      <c r="B12" s="3"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="B13" s="4"/>
-      <c r="K13" s="5"/>
+      <c r="B13" s="3"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="4"/>
-      <c r="K14" s="5"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="B15" s="4"/>
-      <c r="K15" s="5"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" s="4"/>
-      <c r="K16" s="5"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="B17" s="4"/>
-      <c r="K17" s="5"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="4"/>
-      <c r="K18" s="5"/>
+      <c r="B18" s="3"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="4"/>
-      <c r="K19" s="5"/>
+      <c r="B19" s="3"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="4"/>
-      <c r="K20" s="5"/>
+      <c r="B20" s="3"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="4"/>
-      <c r="K21" s="5"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="4"/>
-      <c r="K22" s="5"/>
+      <c r="B22" s="3"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="4"/>
-      <c r="K23" s="5"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="4"/>
-      <c r="K24" s="5"/>
+      <c r="B24" s="3"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="4"/>
-      <c r="K25" s="5"/>
+      <c r="B25" s="3"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="4"/>
-      <c r="K26" s="5"/>
+      <c r="B26" s="3"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="4"/>
-      <c r="K27" s="5"/>
+      <c r="B27" s="3"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="4"/>
-      <c r="K28" s="5"/>
+      <c r="B28" s="3"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="4"/>
-      <c r="K29" s="5"/>
+      <c r="B29" s="3"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="4"/>
-      <c r="K30" s="5"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="4"/>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="4"/>
-      <c r="K32" s="5"/>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="4"/>
-      <c r="K33" s="5"/>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="B34" s="4"/>
-      <c r="K34" s="5"/>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="B35" s="4"/>
-      <c r="K35" s="5"/>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="B36" s="4"/>
-      <c r="K36" s="5"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="B37" s="4"/>
-      <c r="K37" s="5"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="8"/>
-    </row>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
     <row r="39" ht="15.75" customHeight="1"/>
     <row r="40" ht="15.75" customHeight="1"/>
     <row r="41" ht="15.75" customHeight="1"/>
@@ -1862,7 +1782,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B4:K38"/>
+    <mergeCell ref="B4:K31"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -1876,7 +1796,6 @@
   <sheetPr>
     <tabColor rgb="FFFCE5CD"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1888,306 +1807,306 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="27.88"/>
     <col customWidth="1" min="3" max="4" width="21.88"/>
-    <col customWidth="1" min="5" max="6" width="21.13"/>
+    <col customWidth="1" min="5" max="6" width="21.25"/>
     <col customWidth="1" min="23" max="23" width="17.0"/>
-    <col customWidth="1" min="24" max="24" width="17.63"/>
+    <col customWidth="1" min="24" max="24" width="26.5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.0" customHeight="1">
-      <c r="A1" s="9" t="s">
+    <row r="1">
+      <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="13" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="9" t="s">
+      <c r="P1" s="6"/>
+      <c r="Q1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="9" t="s">
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="11"/>
-      <c r="W1" s="12" t="s">
+      <c r="V1" s="6"/>
+      <c r="W1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="12" t="s">
+      <c r="X1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="81.0" customHeight="1">
-      <c r="A2" s="14" t="s">
+    <row r="2">
+      <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="O2" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="Y2" s="15"/>
-    </row>
-    <row r="3" ht="124.5" customHeight="1">
-      <c r="A3" s="16" t="s">
+      <c r="Y2" s="13"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="O3" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="Q3" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="T3" s="16" t="s">
+      <c r="T3" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="18" t="s">
+      <c r="U3" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="V3" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="W3" s="16" t="s">
+      <c r="W3" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="X3" s="19" t="s">
+      <c r="X3" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="Y3" s="20"/>
-    </row>
-    <row r="4" ht="15.0" customHeight="1">
-      <c r="U4" s="21"/>
-      <c r="V4" s="21"/>
-      <c r="X4" s="21"/>
-    </row>
-    <row r="5" ht="15.0" customHeight="1">
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="X5" s="21"/>
-    </row>
-    <row r="6" ht="15.0" customHeight="1">
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="X6" s="21"/>
-    </row>
-    <row r="7" ht="15.0" customHeight="1">
-      <c r="U7" s="21"/>
-      <c r="V7" s="21"/>
-      <c r="X7" s="21"/>
-    </row>
-    <row r="8" ht="15.0" customHeight="1">
-      <c r="U8" s="21"/>
-      <c r="V8" s="21"/>
-      <c r="X8" s="21"/>
-    </row>
-    <row r="9" ht="15.0" customHeight="1">
-      <c r="U9" s="21"/>
-      <c r="V9" s="21"/>
-      <c r="X9" s="21"/>
-    </row>
-    <row r="10" ht="15.0" customHeight="1">
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="X10" s="21"/>
-    </row>
-    <row r="11" ht="15.0" customHeight="1">
-      <c r="U11" s="21"/>
-      <c r="V11" s="21"/>
-      <c r="X11" s="21"/>
-    </row>
-    <row r="12" ht="15.0" customHeight="1">
-      <c r="U12" s="21"/>
-      <c r="V12" s="21"/>
-      <c r="X12" s="21"/>
-    </row>
-    <row r="13" ht="15.0" customHeight="1">
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="X13" s="21"/>
-    </row>
-    <row r="14" ht="15.0" customHeight="1">
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="X14" s="21"/>
-    </row>
-    <row r="15" ht="15.0" customHeight="1">
-      <c r="U15" s="21"/>
-      <c r="V15" s="21"/>
-      <c r="X15" s="21"/>
-    </row>
-    <row r="16" ht="15.0" customHeight="1">
-      <c r="U16" s="21"/>
-      <c r="V16" s="21"/>
-      <c r="X16" s="21"/>
-    </row>
-    <row r="17" ht="15.0" customHeight="1">
-      <c r="U17" s="21"/>
-      <c r="V17" s="21"/>
-      <c r="X17" s="21"/>
-    </row>
-    <row r="18" ht="15.0" customHeight="1">
-      <c r="U18" s="21"/>
-      <c r="V18" s="21"/>
-      <c r="X18" s="21"/>
-    </row>
-    <row r="19" ht="15.0" customHeight="1">
-      <c r="U19" s="21"/>
-      <c r="V19" s="21"/>
-      <c r="X19" s="21"/>
-    </row>
-    <row r="20" ht="15.0" customHeight="1">
-      <c r="U20" s="21"/>
-      <c r="V20" s="21"/>
-      <c r="X20" s="21"/>
-    </row>
-    <row r="21" ht="15.0" customHeight="1">
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="X21" s="21"/>
-    </row>
-    <row r="22" ht="15.0" customHeight="1">
-      <c r="U22" s="21"/>
-      <c r="V22" s="21"/>
-      <c r="X22" s="21"/>
-    </row>
-    <row r="23" ht="15.0" customHeight="1">
-      <c r="U23" s="21"/>
-      <c r="V23" s="21"/>
-      <c r="X23" s="21"/>
+      <c r="Y3" s="17"/>
+    </row>
+    <row r="4">
+      <c r="U4" s="18"/>
+      <c r="V4" s="18"/>
+      <c r="X4" s="19"/>
+    </row>
+    <row r="5">
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="X5" s="19"/>
+    </row>
+    <row r="6">
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="X6" s="19"/>
+    </row>
+    <row r="7">
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="X7" s="19"/>
+    </row>
+    <row r="8">
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="X8" s="19"/>
+    </row>
+    <row r="9">
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="X9" s="19"/>
+    </row>
+    <row r="10">
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="X10" s="19"/>
+    </row>
+    <row r="11">
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="X11" s="19"/>
+    </row>
+    <row r="12">
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="X12" s="19"/>
+    </row>
+    <row r="13">
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="X13" s="19"/>
+    </row>
+    <row r="14">
+      <c r="U14" s="18"/>
+      <c r="V14" s="18"/>
+      <c r="X14" s="19"/>
+    </row>
+    <row r="15">
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="X15" s="19"/>
+    </row>
+    <row r="16">
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="X16" s="19"/>
+    </row>
+    <row r="17">
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="X17" s="19"/>
+    </row>
+    <row r="18">
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="X18" s="19"/>
+    </row>
+    <row r="19">
+      <c r="U19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="X19" s="19"/>
+    </row>
+    <row r="20">
+      <c r="U20" s="18"/>
+      <c r="V20" s="18"/>
+      <c r="X20" s="19"/>
+    </row>
+    <row r="21">
+      <c r="U21" s="18"/>
+      <c r="V21" s="18"/>
+      <c r="X21" s="19"/>
+    </row>
+    <row r="22">
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+      <c r="X22" s="19"/>
+    </row>
+    <row r="23">
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+      <c r="X23" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2198,19 +2117,16 @@
     <mergeCell ref="U1:V1"/>
   </mergeCells>
   <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X4:X23">
+      <formula1>"Choose an option,Keep as-is,Keep but make changes,Merge with other named content,Keep but move elsewhere,Archive,Delete"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U4:U23">
       <formula1>"Yes,Mostly,Some,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X4:X23">
-      <formula1>"Choose an option,Keep as-is,Keep but make changes,Merge with other named content,Keep but move elsewhere,Archive,Delete"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="V4:V23">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>